<commit_message>
objects maping done, input data's diagonal is big_m, added test sheet to excel
</commit_message>
<xml_diff>
--- a/test_sheet.xlsx
+++ b/test_sheet.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khash\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="BadSheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>u1</t>
   </si>
@@ -36,13 +33,61 @@
   </si>
   <si>
     <t>u4</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>dfsf</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>23g</t>
+  </si>
+  <si>
+    <t>gdf</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>gsdf</t>
+  </si>
+  <si>
+    <t>arkusz z blednymi danymi - do testow</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +95,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,10 +412,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -384,13 +439,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D2">
-        <v>42</v>
+        <v>378</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -398,16 +453,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>54</v>
+        <v>486</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -415,16 +470,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>378</v>
       </c>
       <c r="C4">
-        <v>54</v>
+        <v>486</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>65</v>
+        <v>585</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -432,16 +487,352 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>65</v>
+        <v>585</v>
       </c>
       <c r="E5">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9999999</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>9999999</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>9999999</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>9999999</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>9999999</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>9999999</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>9999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>9213509123589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>